<commit_message>
Lasso regression + normalization +lag 1 accuracy results updated
</commit_message>
<xml_diff>
--- a/41108.xlsx
+++ b/41108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A114E21-291D-224F-8D24-4772CAC3321C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B1383-DF58-AB42-A175-483877228890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="4140" windowWidth="27840" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
+    <workbookView xWindow="12740" yWindow="1960" windowWidth="27840" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,10 @@
   </si>
   <si>
     <t>Accuracy(41108)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lasso Regression+normalization+ lag1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -166,12 +170,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -180,6 +178,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C087ABF-8DBB-874F-887F-3BA55E61FC86}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -508,106 +512,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>-667.43322591444598</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>63.694081359801999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>77.520144139150702</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>77.074776640014207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
         <v>-273.85325356476699</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
         <v>77.520144139150702</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="4">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
         <v>74.736648783412605</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="4">
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
         <v>49.7656108508356</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" thickBot="1">
-      <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:3" ht="17" thickBot="1">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="5">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
         <v>62.5372804024381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modification of data preprocessing
</commit_message>
<xml_diff>
--- a/41108.xlsx
+++ b/41108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8EC013-A0FF-3C48-8204-FD07867B67E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2B26F2-6C7D-3848-A352-258A02E72912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="3320" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
+    <workbookView xWindow="3540" yWindow="1420" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -539,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>-667.43322591444598</v>
+        <v>-670.23383041305397</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>63.694081359801999</v>
+        <v>63.765347125414202</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -583,7 +583,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>85.044508627085506</v>
+        <v>84.203732293872307</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
Decision_tree with embedded features
</commit_message>
<xml_diff>
--- a/41108.xlsx
+++ b/41108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2B26F2-6C7D-3848-A352-258A02E72912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E153B437-7B7C-0148-8255-041C59634765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1420" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
+    <workbookView xWindow="11440" yWindow="1440" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,10 @@
   </si>
   <si>
     <t>Lasso Regression+normalization+ lag1 +PCA(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decision Tree Regression+feature selection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C087ABF-8DBB-874F-887F-3BA55E61FC86}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -630,14 +634,25 @@
         <v>49.7656108508356</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" thickBot="1">
-      <c r="A12" s="3">
+    <row r="12" spans="1:3">
+      <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2">
+        <v>85.461516214202803</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" thickBot="1">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>62.5372804024381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final report and final report update
</commit_message>
<xml_diff>
--- a/41108.xlsx
+++ b/41108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39591C99-C220-A548-91A0-48E82231C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D257E35-16D1-6C4C-AEF7-AF7072BF7B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1200" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
+    <workbookView xWindow="400" yWindow="1920" windowWidth="15500" windowHeight="16740" xr2:uid="{DF8DF8F6-78A7-7B4A-84EC-01371F60DB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>